<commit_message>
applicato il de-lombok per problemi al auto-completion
</commit_message>
<xml_diff>
--- a/dati/Fattura_Templ.xlsx
+++ b/dati/Fattura_Templ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\java\photon2\readfatt\dati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9FD637-B9FE-4301-8697-9A19709E9DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DBD503-F6A3-45C3-8FF5-29C1F68098A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22560" yWindow="165" windowWidth="15990" windowHeight="13740" xr2:uid="{E2A2D887-50C5-4B18-AB6F-B16D4B16A3D5}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="17475" windowHeight="18825" xr2:uid="{E2A2D887-50C5-4B18-AB6F-B16D4B16A3D5}"/>
   </bookViews>
   <sheets>
     <sheet name="01-05_31-08-21" sheetId="1" r:id="rId1"/>
@@ -387,13 +387,13 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -711,7 +711,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,7 +834,7 @@
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
-      <c r="L4" s="55"/>
+      <c r="L4" s="53"/>
     </row>
     <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
@@ -877,10 +877,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="54"/>
+      <c r="B6" s="55"/>
       <c r="C6" s="44">
         <v>44347</v>
       </c>

</xml_diff>

<commit_message>
verificato credito anno prec
</commit_message>
<xml_diff>
--- a/dati/Fattura_Templ.xlsx
+++ b/dati/Fattura_Templ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\java\photon2\readfatt\dati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DBD503-F6A3-45C3-8FF5-29C1F68098A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B9F851-C601-4FE3-AADE-80585017E766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="17475" windowHeight="18825" xr2:uid="{E2A2D887-50C5-4B18-AB6F-B16D4B16A3D5}"/>
+    <workbookView xWindow="-33990" yWindow="2160" windowWidth="16935" windowHeight="18180" xr2:uid="{E2A2D887-50C5-4B18-AB6F-B16D4B16A3D5}"/>
   </bookViews>
   <sheets>
     <sheet name="01-05_31-08-21" sheetId="1" r:id="rId1"/>
@@ -711,7 +711,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,6 +721,7 @@
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -895,7 +896,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="9">
-        <f>I2</f>
+        <f>IF(I3-F6&gt;0,I3-F6,0)</f>
         <v>0</v>
       </c>
       <c r="H6" s="3">
@@ -945,7 +946,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="9">
-        <f>IF(G6-F6&gt;0,G6-F6,0)</f>
+        <f>IF(G6-F7&gt;0,G6-F7,0)</f>
         <v>0</v>
       </c>
       <c r="H7" s="8">
@@ -995,7 +996,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="9">
-        <f t="shared" ref="G8:G9" si="9">IF(G7-F7&gt;0,G7-F7,0)</f>
+        <f t="shared" ref="G8:G10" si="9">IF(G7-F8&gt;0,G7-F8,0)</f>
         <v>0</v>
       </c>
       <c r="H8" s="8">
@@ -1095,19 +1096,19 @@
         <v>0</v>
       </c>
       <c r="G10" s="9">
-        <f t="shared" ref="G10" si="10">IF(G9-F9&gt;0,G9-F9,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H10" s="10">
-        <f t="shared" ref="H10" si="11">IF(F10-G10&gt;0,F10-G10,0)</f>
+        <f t="shared" ref="H10" si="10">IF(F10-G10&gt;0,F10-G10,0)</f>
         <v>0</v>
       </c>
       <c r="I10" s="23">
-        <f t="shared" ref="I10" si="12">IF(H10&lt;$K$2,H10,$K$2)</f>
+        <f t="shared" ref="I10" si="11">IF(H10&lt;$K$2,H10,$K$2)</f>
         <v>0</v>
       </c>
       <c r="J10" s="11">
-        <f t="shared" ref="J10" si="13">H10-I10</f>
+        <f t="shared" ref="J10" si="12">H10-I10</f>
         <v>0</v>
       </c>
       <c r="K10" s="26">
@@ -1115,15 +1116,15 @@
         <v>0</v>
       </c>
       <c r="L10" s="24">
-        <f t="shared" ref="L10" si="14">I10*$L$2</f>
+        <f t="shared" ref="L10" si="13">I10*$L$2</f>
         <v>0</v>
       </c>
       <c r="M10" s="24">
-        <f t="shared" ref="M10" si="15">J10*$L$3</f>
+        <f t="shared" ref="M10" si="14">J10*$L$3</f>
         <v>0</v>
       </c>
       <c r="N10" s="33">
-        <f t="shared" ref="N10" si="16">F10*$N$2</f>
+        <f t="shared" ref="N10" si="15">F10*$N$2</f>
         <v>0</v>
       </c>
     </row>
@@ -1132,11 +1133,11 @@
         <v>19</v>
       </c>
       <c r="K12" s="15">
-        <f t="shared" ref="K12:L12" si="17">SUM(K6:K10)</f>
+        <f t="shared" ref="K12:L12" si="16">SUM(K6:K10)</f>
         <v>0</v>
       </c>
       <c r="L12" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="M12" s="15">

</xml_diff>